<commit_message>
Add downloads & how to pages
</commit_message>
<xml_diff>
--- a/data/source.xlsx
+++ b/data/source.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\master\CilioGenics-website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07E819E-7BA9-49D0-8753-98DA64444CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D704062D-A6E8-4FE1-ADB9-B70EE2A2201C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10710" yWindow="2595" windowWidth="15780" windowHeight="12690" xr2:uid="{CBE66C20-32AE-41CA-B07F-26E5F7011757}"/>
+    <workbookView xWindow="1500" yWindow="1860" windowWidth="21750" windowHeight="12690" xr2:uid="{CBE66C20-32AE-41CA-B07F-26E5F7011757}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,28 +84,28 @@
     <t>MotifMap</t>
   </si>
   <si>
+    <t>OMIM</t>
+  </si>
+  <si>
+    <t>https://omim.org/</t>
+  </si>
+  <si>
+    <t>BioMart</t>
+  </si>
+  <si>
+    <t>http://www.ensembl.org/biomart/martview/</t>
+  </si>
+  <si>
+    <t>NCBI</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/</t>
+  </si>
+  <si>
+    <t>ALLIANCE of GENOME RESOURCES</t>
+  </si>
+  <si>
     <t>http://motifmap.ics.uci.edu/</t>
-  </si>
-  <si>
-    <t>OMIM</t>
-  </si>
-  <si>
-    <t>https://omim.org/</t>
-  </si>
-  <si>
-    <t>BioMart</t>
-  </si>
-  <si>
-    <t>http://www.ensembl.org/biomart/martview/</t>
-  </si>
-  <si>
-    <t>NCBI</t>
-  </si>
-  <si>
-    <t>https://www.ncbi.nlm.nih.gov/</t>
-  </si>
-  <si>
-    <t>ALLIANCE of GENOME RESOURCES</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,48 +558,48 @@
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>5</v>
@@ -615,6 +615,8 @@
     <hyperlink ref="B4" r:id="rId3" display="https://pubmed.ncbi.nlm.nih.gov/33958799/" xr:uid="{7566DDB9-1F3E-4948-8360-218130E70408}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{531B8FD7-750E-4709-A96F-E54B2CE69798}"/>
     <hyperlink ref="B5" r:id="rId5" display="https://pubmed.ncbi.nlm.nih.gov/30554520/" xr:uid="{0C0D1887-11B4-46AE-AC5D-A5722CF6C768}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{D5F373BB-5E90-4178-8491-8477D9C5792A}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{6CF2200E-F676-47E7-882E-45FD3A764B3D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix bugs, add text
</commit_message>
<xml_diff>
--- a/data/source.xlsx
+++ b/data/source.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\master\CilioGenics-website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D704062D-A6E8-4FE1-ADB9-B70EE2A2201C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D32374-95D1-448B-AA87-0895E7EE0D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1860" windowWidth="21750" windowHeight="12690" xr2:uid="{CBE66C20-32AE-41CA-B07F-26E5F7011757}"/>
+    <workbookView xWindow="0" yWindow="255" windowWidth="21600" windowHeight="12690" xr2:uid="{CBE66C20-32AE-41CA-B07F-26E5F7011757}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>IntAct</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>http://motifmap.ics.uci.edu/</t>
+  </si>
+  <si>
+    <t>THE HUMAN PROTEIN ATLAS</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/</t>
   </si>
 </sst>
 </file>
@@ -468,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C7DD01D-E83D-4FE9-9BFF-E862B1368333}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,6 +612,14 @@
       </c>
       <c r="C12" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>